<commit_message>
Add G change in "Cofee Ticket Summary", and uproad its sequence and image.
</commit_message>
<xml_diff>
--- a/01_document/04_ソフトウェア実装プロセス/01_ソフトウェア要件定義/03_コーヒーチケット集計.xlsx
+++ b/01_document/04_ソフトウェア実装プロセス/01_ソフトウェア要件定義/03_コーヒーチケット集計.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="150">
   <si>
     <t>コーヒーチケット集計</t>
     <rPh sb="8" eb="10">
@@ -1155,16 +1155,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ユーザー月額料金</t>
-    <rPh sb="4" eb="6">
-      <t>ゲツガク</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>リョウキン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ドルチェグスト</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1678,6 +1668,73 @@
     <t>画面イメージ(改訂F-1)</t>
     <rPh sb="0" eb="2">
       <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>改訂G</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>改訂漏れ</t>
+    <rPh sb="0" eb="2">
+      <t>カイテイ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[コーヒーチケット集計]
+ユーザー月額料金
+</t>
+    <rPh sb="9" eb="11">
+      <t>シュウケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[コーヒーチケット集計]
+ユーザー使用料金
+→今月の料金と同義となってしまうので、誤記修正。
+</t>
+    <rPh sb="9" eb="11">
+      <t>シュウケイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>リョウキン</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>コンゲツ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>リョウキン</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ドウギ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ゴキ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザー使用料金(改訂G-1)</t>
+    <rPh sb="4" eb="6">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>リョウキン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カイテイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1955,6 +2012,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1963,9 +2023,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2487,8 +2544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2538,7 +2595,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -2816,16 +2873,16 @@
         <v>18</v>
       </c>
       <c r="C30" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>100</v>
-      </c>
       <c r="E30" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.15">
@@ -2834,16 +2891,16 @@
         <v>19</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.15">
@@ -2852,16 +2909,16 @@
         <v>20</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
@@ -2870,16 +2927,16 @@
         <v>21</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.15">
@@ -2921,7 +2978,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>26</v>
@@ -2936,7 +2993,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>26</v>
@@ -2960,7 +3017,7 @@
         <v>23</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
@@ -2968,8 +3025,8 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>95</v>
+      <c r="C41" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>25</v>
@@ -2978,7 +3035,7 @@
         <v>23</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
@@ -3151,7 +3208,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C58" s="30" t="b">
+      <c r="C58" s="31" t="b">
         <v>0</v>
       </c>
       <c r="D58" s="6" t="b">
@@ -3165,8 +3222,8 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C59" s="30"/>
-      <c r="D59" s="30" t="b">
+      <c r="C59" s="31"/>
+      <c r="D59" s="31" t="b">
         <v>0</v>
       </c>
       <c r="E59" s="6" t="b">
@@ -3177,8 +3234,8 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
       <c r="E60" s="6" t="b">
         <v>0</v>
       </c>
@@ -3187,7 +3244,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C61" s="30"/>
+      <c r="C61" s="31"/>
       <c r="D61" s="1" t="s">
         <v>53</v>
       </c>
@@ -3195,7 +3252,7 @@
       <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C62" s="30"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="6" t="b">
         <v>1</v>
       </c>
@@ -3213,25 +3270,25 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B66" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C66" s="16"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B68" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C68" s="16"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B70" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C70" s="16"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -3243,7 +3300,7 @@
     <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="16"/>
       <c r="B74" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C74" s="21"/>
       <c r="D74" s="14"/>
@@ -3255,7 +3312,7 @@
       <c r="A75" s="16"/>
       <c r="B75" s="21"/>
       <c r="C75" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
@@ -3273,7 +3330,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -3285,7 +3342,7 @@
     <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" s="16"/>
       <c r="B78" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="14"/>
@@ -3297,7 +3354,7 @@
       <c r="A79" s="16"/>
       <c r="B79" s="16"/>
       <c r="C79" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3401,7 +3458,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3413,10 +3470,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G9"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3430,21 +3487,21 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B2" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" s="25"/>
@@ -3452,30 +3509,30 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B4" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="25">
         <v>11</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="27">
         <v>42859</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
@@ -3484,16 +3541,16 @@
         <v>12</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="27">
         <v>42859</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -3502,16 +3559,16 @@
         <v>13</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="27">
         <v>42859</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="67.5" x14ac:dyDescent="0.15">
@@ -3520,56 +3577,76 @@
         <v>14</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" s="27">
         <v>42859</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="B8" s="33" t="s">
-        <v>137</v>
+      <c r="B8" s="30" t="s">
+        <v>136</v>
       </c>
       <c r="C8" s="25">
         <v>1</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="27">
         <v>42926</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="B9" s="33" t="s">
-        <v>141</v>
+      <c r="B9" s="30" t="s">
+        <v>140</v>
       </c>
       <c r="C9" s="25">
         <v>1</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" s="27">
         <v>42935</v>
       </c>
       <c r="F9" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="G9" s="28" t="s">
-        <v>144</v>
+    </row>
+    <row r="10" spans="2:7" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="B10" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="25">
+        <v>1</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="27">
+        <v>42937</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>